<commit_message>
Idk viele kleine changes
</commit_message>
<xml_diff>
--- a/AlgoPerf.xlsx
+++ b/AlgoPerf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hayla\Desktop\Diplomarbeit\Diplomschrift\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A6A831-BF3F-46AE-B95E-470F7FA6C0E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D611961-834D-4F7B-A312-D92546982C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{EAEC9E2F-F2BC-47B5-9C8B-3D6F6BFF9C1D}"/>
   </bookViews>
@@ -142,7 +142,7 @@
               <a:rPr lang="de-DE" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Performance bei vielen Gegenständen</a:t>
+              <a:t>Dauer bei vielen Gegenständen</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -398,6 +398,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Gegenstände</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -460,6 +515,68 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Gebrauchte Zeit in ms</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1472,7 +1589,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="de-DE" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
-              <a:t>Performance bei vielen Iterationen</a:t>
+              <a:t>Dauer bei vielen Iterationen</a:t>
             </a:r>
             <a:endParaRPr lang="de-DE"/>
           </a:p>
@@ -6544,15 +6661,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>212725</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>92075</xdr:rowOff>
+      <xdr:colOff>754514</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>16341</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>212725</xdr:colOff>
+      <xdr:colOff>754514</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>73025</xdr:rowOff>
+      <xdr:rowOff>183713</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6616,15 +6733,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>597716</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>9088</xdr:rowOff>
+      <xdr:colOff>760835</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>143079</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>590725</xdr:colOff>
+      <xdr:colOff>753844</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>142379</xdr:rowOff>
+      <xdr:rowOff>89948</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6972,7 +7089,7 @@
   <dimension ref="C2:M529"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
-      <selection activeCell="P30" sqref="P30"/>
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>